<commit_message>
Lab 4.7.1 finished, but there is missing point (point 9 in book). I can't add that because there wasn't proper measurements. Lab 4.4.3 fixed mistake with graph.
</commit_message>
<xml_diff>
--- a/Physics/4.7.1/4.7.1.xlsx
+++ b/Physics/4.7.1/4.7.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MIPT-MIPS\Labs\Physics\4.7.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08FCD607-5CB6-4E9D-B02E-FF26872FBD1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06774D6F-487A-4EA6-8AD6-D1A85F62F9F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{457D556B-4563-4964-837B-4E2AD99EB457}"/>
+    <workbookView xWindow="32280" yWindow="3345" windowWidth="29040" windowHeight="15720" xr2:uid="{457D556B-4563-4964-837B-4E2AD99EB457}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>а1</t>
   </si>
@@ -79,12 +79,103 @@
   <si>
     <t>sin \phi_{2e}</t>
   </si>
+  <si>
+    <t>n_o</t>
+  </si>
+  <si>
+    <t>n_e</t>
+  </si>
+  <si>
+    <t>cos^2\theta_o</t>
+  </si>
+  <si>
+    <t>cos^2\theta_e</t>
+  </si>
+  <si>
+    <r>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>ϕ₁</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>180 + Ψ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>ₑ</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>180 + Ψ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>ₒ</t>
+    </r>
+  </si>
+  <si>
+    <t>nₒ</t>
+  </si>
+  <si>
+    <t>nₑ</t>
+  </si>
+  <si>
+    <r>
+      <t>cos^2(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>θ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7.7"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>)ₒ</t>
+    </r>
+  </si>
+  <si>
+    <t>cos^2(θ)ₑ</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,6 +183,20 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="7.7"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -102,7 +207,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -178,11 +283,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -193,6 +313,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -507,10 +648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DA34D78-C0D1-4233-BAE1-7C57BCFAC912}">
-  <dimension ref="A1:AA29"/>
+  <dimension ref="A1:AD62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="Z2" sqref="Z2"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -518,9 +659,14 @@
     <col min="1" max="1" width="11.54296875" customWidth="1"/>
     <col min="8" max="8" width="11.81640625" customWidth="1"/>
     <col min="9" max="9" width="10.6328125" customWidth="1"/>
+    <col min="17" max="17" width="11.54296875" customWidth="1"/>
+    <col min="18" max="18" width="12.08984375" customWidth="1"/>
+    <col min="19" max="19" width="15.1796875" customWidth="1"/>
+    <col min="29" max="29" width="13.81640625" customWidth="1"/>
+    <col min="30" max="30" width="14.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.35">
       <c r="G1" t="s">
         <v>4</v>
       </c>
@@ -551,8 +697,20 @@
       <c r="S1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="Z1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -623,8 +781,16 @@
         <f>Y2*1.66</f>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="AC2">
+        <f>(Q2/Z2)*Q2/Z2</f>
+        <v>0</v>
+      </c>
+      <c r="AD2" t="e">
+        <f>(Q2/AA2)*Q2/AA2</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.35">
       <c r="B3">
         <v>320</v>
       </c>
@@ -700,8 +866,16 @@
         <f t="shared" ref="AA3:AA29" si="12">Y3*1.66</f>
         <v>1.6307948080826942</v>
       </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="AC3">
+        <f t="shared" ref="AC3:AC29" si="13">(Q3/Z3)*Q3/Z3</f>
+        <v>5.7243338909505751E-4</v>
+      </c>
+      <c r="AD3">
+        <f>(Q3/AA3)*Q3/AA3</f>
+        <v>4.5750876327600043E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -776,8 +950,16 @@
         <f t="shared" si="12"/>
         <v>1.6147278283706492</v>
       </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="AC4">
+        <f t="shared" si="13"/>
+        <v>2.9271632494868292E-3</v>
+      </c>
+      <c r="AD4">
+        <f t="shared" ref="AD3:AD29" si="14">(Q4/AA4)*Q4/AA4</f>
+        <v>2.3585679520357022E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
       <c r="G5">
         <v>15</v>
       </c>
@@ -839,8 +1021,16 @@
         <f t="shared" si="12"/>
         <v>1.6370157692912335</v>
       </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="AC5">
+        <f t="shared" si="13"/>
+        <v>8.0199704794082765E-3</v>
+      </c>
+      <c r="AD5">
+        <f t="shared" si="14"/>
+        <v>6.3511399036192424E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.35">
       <c r="G6">
         <v>20</v>
       </c>
@@ -902,8 +1092,16 @@
         <f t="shared" si="12"/>
         <v>1.6264426785103034</v>
       </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="AC6">
+        <f t="shared" si="13"/>
+        <v>1.4452156951793553E-2</v>
+      </c>
+      <c r="AD6">
+        <f t="shared" si="14"/>
+        <v>1.1387462667923828E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
       <c r="G7">
         <v>25</v>
       </c>
@@ -965,8 +1163,16 @@
         <f t="shared" si="12"/>
         <v>1.6089108946950075</v>
       </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="AC7">
+        <f t="shared" si="13"/>
+        <v>2.2323375363903671E-2</v>
+      </c>
+      <c r="AD7">
+        <f t="shared" si="14"/>
+        <v>1.8079069472305767E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.35">
       <c r="G8">
         <v>30</v>
       </c>
@@ -1028,8 +1234,16 @@
         <f t="shared" si="12"/>
         <v>1.6025396663995981</v>
       </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="AC8">
+        <f t="shared" si="13"/>
+        <v>3.267294715382308E-2</v>
+      </c>
+      <c r="AD8">
+        <f t="shared" si="14"/>
+        <v>2.6058207590114426E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.35">
       <c r="G9">
         <v>35</v>
       </c>
@@ -1091,8 +1305,16 @@
         <f t="shared" si="12"/>
         <v>1.5929661238164967</v>
       </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="AC9">
+        <f t="shared" si="13"/>
+        <v>4.3950010544162796E-2</v>
+      </c>
+      <c r="AD9">
+        <f t="shared" si="14"/>
+        <v>3.5599496368201811E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.35">
       <c r="C10">
         <v>21</v>
       </c>
@@ -1163,8 +1385,16 @@
         <f t="shared" si="12"/>
         <v>1.5804237295970429</v>
       </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="AC10">
+        <f t="shared" si="13"/>
+        <v>5.8455541953607533E-2</v>
+      </c>
+      <c r="AD10">
+        <f t="shared" si="14"/>
+        <v>4.6787933423951052E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
       <c r="C11">
         <v>30</v>
       </c>
@@ -1235,8 +1465,16 @@
         <f t="shared" si="12"/>
         <v>1.5864519958260412</v>
       </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="AC11">
+        <f t="shared" si="13"/>
+        <v>7.6147050527534524E-2</v>
+      </c>
+      <c r="AD11">
+        <f t="shared" si="14"/>
+        <v>6.0601811684994074E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.35">
       <c r="C12">
         <v>35</v>
       </c>
@@ -1307,8 +1545,16 @@
         <f t="shared" si="12"/>
         <v>1.5686875345914901</v>
       </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="AC12">
+        <f t="shared" si="13"/>
+        <v>8.9010263003729356E-2</v>
+      </c>
+      <c r="AD12">
+        <f t="shared" si="14"/>
+        <v>7.2512266027215153E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.35">
       <c r="C13">
         <v>42</v>
       </c>
@@ -1379,8 +1625,16 @@
         <f t="shared" si="12"/>
         <v>1.5711444297729913</v>
       </c>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="AC13">
+        <f t="shared" si="13"/>
+        <v>0.10620295584979327</v>
+      </c>
+      <c r="AD13">
+        <f t="shared" si="14"/>
+        <v>8.6292463066055911E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.35">
       <c r="C14">
         <v>54</v>
       </c>
@@ -1451,8 +1705,16 @@
         <f t="shared" si="12"/>
         <v>1.5725377656757851</v>
       </c>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="AC14">
+        <f t="shared" si="13"/>
+        <v>0.12453659674202831</v>
+      </c>
+      <c r="AD14">
+        <f t="shared" si="14"/>
+        <v>0.10100395411157649</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.35">
       <c r="C15">
         <v>70</v>
       </c>
@@ -1520,8 +1782,16 @@
         <f t="shared" si="12"/>
         <v>1.5728597822931758</v>
       </c>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="AC15">
+        <f t="shared" si="13"/>
+        <v>0.13939085302256604</v>
+      </c>
+      <c r="AD15">
+        <f t="shared" si="14"/>
+        <v>0.11658987644979844</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.35">
       <c r="G16">
         <v>70</v>
       </c>
@@ -1583,8 +1853,16 @@
         <f t="shared" si="12"/>
         <v>1.5721086887672266</v>
       </c>
-    </row>
-    <row r="17" spans="2:27" x14ac:dyDescent="0.35">
+      <c r="AC16">
+        <f t="shared" si="13"/>
+        <v>0.15906385883699264</v>
+      </c>
+      <c r="AD16">
+        <f t="shared" si="14"/>
+        <v>0.13299434869981294</v>
+      </c>
+    </row>
+    <row r="17" spans="2:30" x14ac:dyDescent="0.35">
       <c r="G17">
         <v>75</v>
       </c>
@@ -1646,8 +1924,16 @@
         <f t="shared" si="12"/>
         <v>1.5702886637165707</v>
       </c>
-    </row>
-    <row r="18" spans="2:27" x14ac:dyDescent="0.35">
+      <c r="AC17">
+        <f t="shared" si="13"/>
+        <v>0.17954476172123551</v>
+      </c>
+      <c r="AD17">
+        <f t="shared" si="14"/>
+        <v>0.15016182775699652</v>
+      </c>
+    </row>
+    <row r="18" spans="2:30" x14ac:dyDescent="0.35">
       <c r="B18">
         <f>SIN(E3)</f>
         <v>0.6015535345767008</v>
@@ -1717,8 +2003,16 @@
         <f t="shared" si="12"/>
         <v>1.5895803283853804</v>
       </c>
-    </row>
-    <row r="19" spans="2:27" x14ac:dyDescent="0.35">
+      <c r="AC18">
+        <f t="shared" si="13"/>
+        <v>0.19466082076598806</v>
+      </c>
+      <c r="AD18">
+        <f t="shared" si="14"/>
+        <v>0.16338174917441289</v>
+      </c>
+    </row>
+    <row r="19" spans="2:30" x14ac:dyDescent="0.35">
       <c r="G19">
         <v>85</v>
       </c>
@@ -1780,8 +2074,16 @@
         <f t="shared" si="12"/>
         <v>1.5855577685573605</v>
       </c>
-    </row>
-    <row r="20" spans="2:27" x14ac:dyDescent="0.35">
+      <c r="AC19">
+        <f t="shared" si="13"/>
+        <v>0.21586424413693955</v>
+      </c>
+      <c r="AD19">
+        <f t="shared" si="14"/>
+        <v>0.18140362737025403</v>
+      </c>
+    </row>
+    <row r="20" spans="2:30" x14ac:dyDescent="0.35">
       <c r="G20">
         <v>90</v>
       </c>
@@ -1843,8 +2145,16 @@
         <f t="shared" si="12"/>
         <v>1.5804237295970429</v>
       </c>
-    </row>
-    <row r="21" spans="2:27" x14ac:dyDescent="0.35">
+      <c r="AC20">
+        <f t="shared" si="13"/>
+        <v>0.23068398491741005</v>
+      </c>
+      <c r="AD20">
+        <f t="shared" si="14"/>
+        <v>0.20002162100458809</v>
+      </c>
+    </row>
+    <row r="21" spans="2:30" x14ac:dyDescent="0.35">
       <c r="G21">
         <v>95</v>
       </c>
@@ -1906,8 +2216,16 @@
         <f t="shared" si="12"/>
         <v>1.5958699362115809</v>
       </c>
-    </row>
-    <row r="22" spans="2:27" x14ac:dyDescent="0.35">
+      <c r="AC21">
+        <f t="shared" si="13"/>
+        <v>0.25229227285153338</v>
+      </c>
+      <c r="AD21">
+        <f t="shared" si="14"/>
+        <v>0.21327115979374317</v>
+      </c>
+    </row>
+    <row r="22" spans="2:30" x14ac:dyDescent="0.35">
       <c r="G22">
         <v>100</v>
       </c>
@@ -1969,8 +2287,16 @@
         <f t="shared" si="12"/>
         <v>1.6097012171819711</v>
       </c>
-    </row>
-    <row r="23" spans="2:27" x14ac:dyDescent="0.35">
+      <c r="AC22">
+        <f t="shared" si="13"/>
+        <v>0.26666219699703231</v>
+      </c>
+      <c r="AD22">
+        <f t="shared" si="14"/>
+        <v>0.22630534162619045</v>
+      </c>
+    </row>
+    <row r="23" spans="2:30" x14ac:dyDescent="0.35">
       <c r="G23">
         <v>105</v>
       </c>
@@ -2032,8 +2358,16 @@
         <f t="shared" si="12"/>
         <v>1.6006336902732912</v>
       </c>
-    </row>
-    <row r="24" spans="2:27" x14ac:dyDescent="0.35">
+      <c r="AC23">
+        <f t="shared" si="13"/>
+        <v>0.28841667191376597</v>
+      </c>
+      <c r="AD23">
+        <f t="shared" si="14"/>
+        <v>0.24549330429356572</v>
+      </c>
+    </row>
+    <row r="24" spans="2:30" x14ac:dyDescent="0.35">
       <c r="G24">
         <v>110</v>
       </c>
@@ -2095,8 +2429,16 @@
         <f t="shared" si="12"/>
         <v>1.611177470171721</v>
       </c>
-    </row>
-    <row r="25" spans="2:27" x14ac:dyDescent="0.35">
+      <c r="AC24">
+        <f t="shared" si="13"/>
+        <v>0.2943918465532504</v>
+      </c>
+      <c r="AD24">
+        <f t="shared" si="14"/>
+        <v>0.2583129335637368</v>
+      </c>
+    </row>
+    <row r="25" spans="2:30" x14ac:dyDescent="0.35">
       <c r="G25">
         <v>115</v>
       </c>
@@ -2158,8 +2500,16 @@
         <f t="shared" si="12"/>
         <v>1.6198093337909325</v>
       </c>
-    </row>
-    <row r="26" spans="2:27" x14ac:dyDescent="0.35">
+      <c r="AC25">
+        <f t="shared" si="13"/>
+        <v>0.30778820015048997</v>
+      </c>
+      <c r="AD25">
+        <f t="shared" si="14"/>
+        <v>0.27092488979724583</v>
+      </c>
+    </row>
+    <row r="26" spans="2:30" x14ac:dyDescent="0.35">
       <c r="G26">
         <v>120</v>
       </c>
@@ -2221,8 +2571,16 @@
         <f t="shared" si="12"/>
         <v>1.6264426785103034</v>
       </c>
-    </row>
-    <row r="27" spans="2:27" x14ac:dyDescent="0.35">
+      <c r="AC26">
+        <f t="shared" si="13"/>
+        <v>0.3209020084529689</v>
+      </c>
+      <c r="AD26">
+        <f t="shared" si="14"/>
+        <v>0.28334617118633443</v>
+      </c>
+    </row>
+    <row r="27" spans="2:30" x14ac:dyDescent="0.35">
       <c r="G27">
         <v>125</v>
       </c>
@@ -2284,8 +2642,16 @@
         <f t="shared" si="12"/>
         <v>1.631000878937972</v>
       </c>
-    </row>
-    <row r="28" spans="2:27" x14ac:dyDescent="0.35">
+      <c r="AC27">
+        <f t="shared" si="13"/>
+        <v>0.33375802536323124</v>
+      </c>
+      <c r="AD27">
+        <f t="shared" si="14"/>
+        <v>0.2955964696913736</v>
+      </c>
+    </row>
+    <row r="28" spans="2:30" x14ac:dyDescent="0.35">
       <c r="G28">
         <v>130</v>
       </c>
@@ -2347,8 +2713,16 @@
         <f t="shared" si="12"/>
         <v>1.6334173365843989</v>
       </c>
-    </row>
-    <row r="29" spans="2:27" x14ac:dyDescent="0.35">
+      <c r="AC28">
+        <f t="shared" si="13"/>
+        <v>0.34638192096621484</v>
+      </c>
+      <c r="AD28">
+        <f t="shared" si="14"/>
+        <v>0.30769751149758773</v>
+      </c>
+    </row>
+    <row r="29" spans="2:30" x14ac:dyDescent="0.35">
       <c r="G29">
         <v>135</v>
       </c>
@@ -2410,8 +2784,1028 @@
         <f t="shared" si="12"/>
         <v>1.6336355658593955</v>
       </c>
+      <c r="AC29">
+        <f t="shared" si="13"/>
+        <v>0.3506952689763535</v>
+      </c>
+      <c r="AD29">
+        <f t="shared" si="14"/>
+        <v>0.31967249668293474</v>
+      </c>
+    </row>
+    <row r="33" spans="5:27" x14ac:dyDescent="0.35">
+      <c r="Z33">
+        <f>AVERAGE(Z2:Z29)</f>
+        <v>1.4643381503853099</v>
+      </c>
+      <c r="AA33">
+        <f>AVERAGE(AA3:AA29)</f>
+        <v>1.6009314923506541</v>
+      </c>
+    </row>
+    <row r="34" spans="5:27" x14ac:dyDescent="0.35">
+      <c r="G34" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="H34" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I34" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="J34" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K34" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="L34" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="M34" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="5:27" x14ac:dyDescent="0.35">
+      <c r="E35">
+        <f>H35-180</f>
+        <v>27</v>
+      </c>
+      <c r="F35" t="e">
+        <f>I35-180</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G35" s="8">
+        <v>0</v>
+      </c>
+      <c r="H35" s="9">
+        <v>207</v>
+      </c>
+      <c r="I35" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="J35" s="8">
+        <f>H35*1.66</f>
+        <v>343.62</v>
+      </c>
+      <c r="K35" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="L35" s="9">
+        <f>AC2</f>
+        <v>0</v>
+      </c>
+      <c r="M35" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="5:27" x14ac:dyDescent="0.35">
+      <c r="E36">
+        <f t="shared" ref="E36:E62" si="15">H36-180</f>
+        <v>24</v>
+      </c>
+      <c r="F36">
+        <f t="shared" ref="F36:F62" si="16">I36-180</f>
+        <v>39</v>
+      </c>
+      <c r="G36" s="10">
+        <v>4</v>
+      </c>
+      <c r="H36" s="11">
+        <v>204</v>
+      </c>
+      <c r="I36" s="11">
+        <v>219</v>
+      </c>
+      <c r="J36" s="10">
+        <f t="shared" ref="J36:J62" si="17">H36*1.66</f>
+        <v>338.64</v>
+      </c>
+      <c r="K36" s="11">
+        <f t="shared" ref="K36:K62" si="18">I36*1.66</f>
+        <v>363.53999999999996</v>
+      </c>
+      <c r="L36" s="11">
+        <f t="shared" ref="L36:M36" si="19">AC3</f>
+        <v>5.7243338909505751E-4</v>
+      </c>
+      <c r="M36" s="11">
+        <f t="shared" si="19"/>
+        <v>4.5750876327600043E-4</v>
+      </c>
+    </row>
+    <row r="37" spans="5:27" x14ac:dyDescent="0.35">
+      <c r="E37">
+        <f t="shared" si="15"/>
+        <v>23</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="16"/>
+        <v>35</v>
+      </c>
+      <c r="G37" s="10">
+        <v>9</v>
+      </c>
+      <c r="H37" s="11">
+        <v>203</v>
+      </c>
+      <c r="I37" s="11">
+        <v>215</v>
+      </c>
+      <c r="J37" s="10">
+        <f t="shared" si="17"/>
+        <v>336.97999999999996</v>
+      </c>
+      <c r="K37" s="11">
+        <f t="shared" si="18"/>
+        <v>356.9</v>
+      </c>
+      <c r="L37" s="11">
+        <f t="shared" ref="L37:M37" si="20">AC4</f>
+        <v>2.9271632494868292E-3</v>
+      </c>
+      <c r="M37" s="11">
+        <f t="shared" si="20"/>
+        <v>2.3585679520357022E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="5:27" x14ac:dyDescent="0.35">
+      <c r="E38">
+        <f t="shared" si="15"/>
+        <v>23</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="16"/>
+        <v>35</v>
+      </c>
+      <c r="G38" s="10">
+        <v>15</v>
+      </c>
+      <c r="H38" s="11">
+        <v>203</v>
+      </c>
+      <c r="I38" s="11">
+        <v>215</v>
+      </c>
+      <c r="J38" s="10">
+        <f t="shared" si="17"/>
+        <v>336.97999999999996</v>
+      </c>
+      <c r="K38" s="11">
+        <f t="shared" si="18"/>
+        <v>356.9</v>
+      </c>
+      <c r="L38" s="11">
+        <f t="shared" ref="L38:M38" si="21">AC5</f>
+        <v>8.0199704794082765E-3</v>
+      </c>
+      <c r="M38" s="11">
+        <f t="shared" si="21"/>
+        <v>6.3511399036192424E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="5:27" x14ac:dyDescent="0.35">
+      <c r="E39">
+        <f t="shared" si="15"/>
+        <v>22</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="16"/>
+        <v>33</v>
+      </c>
+      <c r="G39" s="10">
+        <v>20</v>
+      </c>
+      <c r="H39" s="11">
+        <v>202</v>
+      </c>
+      <c r="I39" s="11">
+        <v>213</v>
+      </c>
+      <c r="J39" s="10">
+        <f t="shared" si="17"/>
+        <v>335.32</v>
+      </c>
+      <c r="K39" s="11">
+        <f t="shared" si="18"/>
+        <v>353.58</v>
+      </c>
+      <c r="L39" s="11">
+        <f t="shared" ref="L39:M39" si="22">AC6</f>
+        <v>1.4452156951793553E-2</v>
+      </c>
+      <c r="M39" s="11">
+        <f t="shared" si="22"/>
+        <v>1.1387462667923828E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="5:27" x14ac:dyDescent="0.35">
+      <c r="E40">
+        <f t="shared" si="15"/>
+        <v>22</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="16"/>
+        <v>31</v>
+      </c>
+      <c r="G40" s="10">
+        <v>25</v>
+      </c>
+      <c r="H40" s="11">
+        <v>202</v>
+      </c>
+      <c r="I40" s="11">
+        <v>211</v>
+      </c>
+      <c r="J40" s="10">
+        <f t="shared" si="17"/>
+        <v>335.32</v>
+      </c>
+      <c r="K40" s="11">
+        <f t="shared" si="18"/>
+        <v>350.26</v>
+      </c>
+      <c r="L40" s="11">
+        <f t="shared" ref="L40:M40" si="23">AC7</f>
+        <v>2.2323375363903671E-2</v>
+      </c>
+      <c r="M40" s="11">
+        <f t="shared" si="23"/>
+        <v>1.8079069472305767E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="5:27" x14ac:dyDescent="0.35">
+      <c r="E41">
+        <f t="shared" si="15"/>
+        <v>21</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="16"/>
+        <v>30</v>
+      </c>
+      <c r="G41" s="10">
+        <v>30</v>
+      </c>
+      <c r="H41" s="11">
+        <v>201</v>
+      </c>
+      <c r="I41" s="11">
+        <v>210</v>
+      </c>
+      <c r="J41" s="10">
+        <f t="shared" si="17"/>
+        <v>333.65999999999997</v>
+      </c>
+      <c r="K41" s="11">
+        <f t="shared" si="18"/>
+        <v>348.59999999999997</v>
+      </c>
+      <c r="L41" s="11">
+        <f t="shared" ref="L41:M41" si="24">AC8</f>
+        <v>3.267294715382308E-2</v>
+      </c>
+      <c r="M41" s="11">
+        <f t="shared" si="24"/>
+        <v>2.6058207590114426E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="5:27" x14ac:dyDescent="0.35">
+      <c r="E42">
+        <f t="shared" si="15"/>
+        <v>21</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="16"/>
+        <v>29</v>
+      </c>
+      <c r="G42" s="10">
+        <v>35</v>
+      </c>
+      <c r="H42" s="11">
+        <v>201</v>
+      </c>
+      <c r="I42" s="11">
+        <v>209</v>
+      </c>
+      <c r="J42" s="10">
+        <f t="shared" si="17"/>
+        <v>333.65999999999997</v>
+      </c>
+      <c r="K42" s="11">
+        <f t="shared" si="18"/>
+        <v>346.94</v>
+      </c>
+      <c r="L42" s="11">
+        <f t="shared" ref="L42:M42" si="25">AC9</f>
+        <v>4.3950010544162796E-2</v>
+      </c>
+      <c r="M42" s="11">
+        <f t="shared" si="25"/>
+        <v>3.5599496368201811E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="5:27" x14ac:dyDescent="0.35">
+      <c r="E43">
+        <f t="shared" si="15"/>
+        <v>20</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="16"/>
+        <v>28</v>
+      </c>
+      <c r="G43" s="10">
+        <v>40</v>
+      </c>
+      <c r="H43" s="11">
+        <v>200</v>
+      </c>
+      <c r="I43" s="11">
+        <v>208</v>
+      </c>
+      <c r="J43" s="10">
+        <f t="shared" si="17"/>
+        <v>332</v>
+      </c>
+      <c r="K43" s="11">
+        <f t="shared" si="18"/>
+        <v>345.28</v>
+      </c>
+      <c r="L43" s="11">
+        <f t="shared" ref="L43:M43" si="26">AC10</f>
+        <v>5.8455541953607533E-2</v>
+      </c>
+      <c r="M43" s="11">
+        <f t="shared" si="26"/>
+        <v>4.6787933423951052E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="5:27" x14ac:dyDescent="0.35">
+      <c r="E44">
+        <f t="shared" si="15"/>
+        <v>20</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="16"/>
+        <v>28</v>
+      </c>
+      <c r="G44" s="10">
+        <v>46</v>
+      </c>
+      <c r="H44" s="11">
+        <v>200</v>
+      </c>
+      <c r="I44" s="11">
+        <v>208</v>
+      </c>
+      <c r="J44" s="10">
+        <f t="shared" si="17"/>
+        <v>332</v>
+      </c>
+      <c r="K44" s="11">
+        <f t="shared" si="18"/>
+        <v>345.28</v>
+      </c>
+      <c r="L44" s="11">
+        <f t="shared" ref="L44:M44" si="27">AC11</f>
+        <v>7.6147050527534524E-2</v>
+      </c>
+      <c r="M44" s="11">
+        <f t="shared" si="27"/>
+        <v>6.0601811684994074E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="5:27" x14ac:dyDescent="0.35">
+      <c r="E45">
+        <f t="shared" si="15"/>
+        <v>20</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="16"/>
+        <v>27</v>
+      </c>
+      <c r="G45" s="10">
+        <v>50</v>
+      </c>
+      <c r="H45" s="11">
+        <v>200</v>
+      </c>
+      <c r="I45" s="11">
+        <v>207</v>
+      </c>
+      <c r="J45" s="10">
+        <f t="shared" si="17"/>
+        <v>332</v>
+      </c>
+      <c r="K45" s="11">
+        <f t="shared" si="18"/>
+        <v>343.62</v>
+      </c>
+      <c r="L45" s="11">
+        <f t="shared" ref="L45:M45" si="28">AC12</f>
+        <v>8.9010263003729356E-2</v>
+      </c>
+      <c r="M45" s="11">
+        <f t="shared" si="28"/>
+        <v>7.2512266027215153E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="5:27" x14ac:dyDescent="0.35">
+      <c r="E46">
+        <f t="shared" si="15"/>
+        <v>20</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="16"/>
+        <v>27</v>
+      </c>
+      <c r="G46" s="10">
+        <v>55</v>
+      </c>
+      <c r="H46" s="11">
+        <v>200</v>
+      </c>
+      <c r="I46" s="11">
+        <v>207</v>
+      </c>
+      <c r="J46" s="10">
+        <f t="shared" si="17"/>
+        <v>332</v>
+      </c>
+      <c r="K46" s="11">
+        <f t="shared" si="18"/>
+        <v>343.62</v>
+      </c>
+      <c r="L46" s="11">
+        <f t="shared" ref="L46:M46" si="29">AC13</f>
+        <v>0.10620295584979327</v>
+      </c>
+      <c r="M46" s="11">
+        <f t="shared" si="29"/>
+        <v>8.6292463066055911E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="5:27" x14ac:dyDescent="0.35">
+      <c r="E47">
+        <f t="shared" si="15"/>
+        <v>20</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="16"/>
+        <v>27</v>
+      </c>
+      <c r="G47" s="10">
+        <v>60</v>
+      </c>
+      <c r="H47" s="11">
+        <v>200</v>
+      </c>
+      <c r="I47" s="11">
+        <v>207</v>
+      </c>
+      <c r="J47" s="10">
+        <f t="shared" si="17"/>
+        <v>332</v>
+      </c>
+      <c r="K47" s="11">
+        <f t="shared" si="18"/>
+        <v>343.62</v>
+      </c>
+      <c r="L47" s="11">
+        <f t="shared" ref="L47:M47" si="30">AC14</f>
+        <v>0.12453659674202831</v>
+      </c>
+      <c r="M47" s="11">
+        <f t="shared" si="30"/>
+        <v>0.10100395411157649</v>
+      </c>
+    </row>
+    <row r="48" spans="5:27" x14ac:dyDescent="0.35">
+      <c r="E48">
+        <f t="shared" si="15"/>
+        <v>21</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="16"/>
+        <v>27</v>
+      </c>
+      <c r="G48" s="10">
+        <v>65</v>
+      </c>
+      <c r="H48" s="11">
+        <v>201</v>
+      </c>
+      <c r="I48" s="11">
+        <v>207</v>
+      </c>
+      <c r="J48" s="10">
+        <f t="shared" si="17"/>
+        <v>333.65999999999997</v>
+      </c>
+      <c r="K48" s="11">
+        <f t="shared" si="18"/>
+        <v>343.62</v>
+      </c>
+      <c r="L48" s="11">
+        <f t="shared" ref="L48:M48" si="31">AC15</f>
+        <v>0.13939085302256604</v>
+      </c>
+      <c r="M48" s="11">
+        <f t="shared" si="31"/>
+        <v>0.11658987644979844</v>
+      </c>
+    </row>
+    <row r="49" spans="5:13" x14ac:dyDescent="0.35">
+      <c r="E49">
+        <f t="shared" si="15"/>
+        <v>21</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="16"/>
+        <v>27</v>
+      </c>
+      <c r="G49" s="10">
+        <v>70</v>
+      </c>
+      <c r="H49" s="11">
+        <v>201</v>
+      </c>
+      <c r="I49" s="11">
+        <v>207</v>
+      </c>
+      <c r="J49" s="10">
+        <f t="shared" si="17"/>
+        <v>333.65999999999997</v>
+      </c>
+      <c r="K49" s="11">
+        <f t="shared" si="18"/>
+        <v>343.62</v>
+      </c>
+      <c r="L49" s="11">
+        <f t="shared" ref="L49:M49" si="32">AC16</f>
+        <v>0.15906385883699264</v>
+      </c>
+      <c r="M49" s="11">
+        <f t="shared" si="32"/>
+        <v>0.13299434869981294</v>
+      </c>
+    </row>
+    <row r="50" spans="5:13" x14ac:dyDescent="0.35">
+      <c r="E50">
+        <f t="shared" si="15"/>
+        <v>21</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="16"/>
+        <v>27</v>
+      </c>
+      <c r="G50" s="10">
+        <v>75</v>
+      </c>
+      <c r="H50" s="11">
+        <v>201</v>
+      </c>
+      <c r="I50" s="11">
+        <v>207</v>
+      </c>
+      <c r="J50" s="10">
+        <f t="shared" si="17"/>
+        <v>333.65999999999997</v>
+      </c>
+      <c r="K50" s="11">
+        <f t="shared" si="18"/>
+        <v>343.62</v>
+      </c>
+      <c r="L50" s="11">
+        <f t="shared" ref="L50:M50" si="33">AC17</f>
+        <v>0.17954476172123551</v>
+      </c>
+      <c r="M50" s="11">
+        <f t="shared" si="33"/>
+        <v>0.15016182775699652</v>
+      </c>
+    </row>
+    <row r="51" spans="5:13" x14ac:dyDescent="0.35">
+      <c r="E51">
+        <f t="shared" si="15"/>
+        <v>22</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="16"/>
+        <v>28</v>
+      </c>
+      <c r="G51" s="10">
+        <v>80</v>
+      </c>
+      <c r="H51" s="11">
+        <v>202</v>
+      </c>
+      <c r="I51" s="11">
+        <v>208</v>
+      </c>
+      <c r="J51" s="10">
+        <f t="shared" si="17"/>
+        <v>335.32</v>
+      </c>
+      <c r="K51" s="11">
+        <f t="shared" si="18"/>
+        <v>345.28</v>
+      </c>
+      <c r="L51" s="11">
+        <f t="shared" ref="L51:M51" si="34">AC18</f>
+        <v>0.19466082076598806</v>
+      </c>
+      <c r="M51" s="11">
+        <f t="shared" si="34"/>
+        <v>0.16338174917441289</v>
+      </c>
+    </row>
+    <row r="52" spans="5:13" x14ac:dyDescent="0.35">
+      <c r="E52">
+        <f t="shared" si="15"/>
+        <v>22</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="16"/>
+        <v>28</v>
+      </c>
+      <c r="G52" s="10">
+        <v>85</v>
+      </c>
+      <c r="H52" s="11">
+        <v>202</v>
+      </c>
+      <c r="I52" s="11">
+        <v>208</v>
+      </c>
+      <c r="J52" s="10">
+        <f t="shared" si="17"/>
+        <v>335.32</v>
+      </c>
+      <c r="K52" s="11">
+        <f t="shared" si="18"/>
+        <v>345.28</v>
+      </c>
+      <c r="L52" s="11">
+        <f t="shared" ref="L52:M52" si="35">AC19</f>
+        <v>0.21586424413693955</v>
+      </c>
+      <c r="M52" s="11">
+        <f t="shared" si="35"/>
+        <v>0.18140362737025403</v>
+      </c>
+    </row>
+    <row r="53" spans="5:13" x14ac:dyDescent="0.35">
+      <c r="E53">
+        <f t="shared" si="15"/>
+        <v>23</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="16"/>
+        <v>28</v>
+      </c>
+      <c r="G53" s="10">
+        <v>90</v>
+      </c>
+      <c r="H53" s="11">
+        <v>203</v>
+      </c>
+      <c r="I53" s="11">
+        <v>208</v>
+      </c>
+      <c r="J53" s="10">
+        <f t="shared" si="17"/>
+        <v>336.97999999999996</v>
+      </c>
+      <c r="K53" s="11">
+        <f t="shared" si="18"/>
+        <v>345.28</v>
+      </c>
+      <c r="L53" s="11">
+        <f t="shared" ref="L53:M53" si="36">AC20</f>
+        <v>0.23068398491741005</v>
+      </c>
+      <c r="M53" s="11">
+        <f t="shared" si="36"/>
+        <v>0.20002162100458809</v>
+      </c>
+    </row>
+    <row r="54" spans="5:13" x14ac:dyDescent="0.35">
+      <c r="E54">
+        <f t="shared" si="15"/>
+        <v>23</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="16"/>
+        <v>29</v>
+      </c>
+      <c r="G54" s="10">
+        <v>95</v>
+      </c>
+      <c r="H54" s="11">
+        <v>203</v>
+      </c>
+      <c r="I54" s="11">
+        <v>209</v>
+      </c>
+      <c r="J54" s="10">
+        <f t="shared" si="17"/>
+        <v>336.97999999999996</v>
+      </c>
+      <c r="K54" s="11">
+        <f t="shared" si="18"/>
+        <v>346.94</v>
+      </c>
+      <c r="L54" s="11">
+        <f t="shared" ref="L54:M54" si="37">AC21</f>
+        <v>0.25229227285153338</v>
+      </c>
+      <c r="M54" s="11">
+        <f t="shared" si="37"/>
+        <v>0.21327115979374317</v>
+      </c>
+    </row>
+    <row r="55" spans="5:13" x14ac:dyDescent="0.35">
+      <c r="E55">
+        <f t="shared" si="15"/>
+        <v>24</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="16"/>
+        <v>30</v>
+      </c>
+      <c r="G55" s="10">
+        <v>100</v>
+      </c>
+      <c r="H55" s="11">
+        <v>204</v>
+      </c>
+      <c r="I55" s="11">
+        <v>210</v>
+      </c>
+      <c r="J55" s="10">
+        <f t="shared" si="17"/>
+        <v>338.64</v>
+      </c>
+      <c r="K55" s="11">
+        <f t="shared" si="18"/>
+        <v>348.59999999999997</v>
+      </c>
+      <c r="L55" s="11">
+        <f t="shared" ref="L55:M55" si="38">AC22</f>
+        <v>0.26666219699703231</v>
+      </c>
+      <c r="M55" s="11">
+        <f t="shared" si="38"/>
+        <v>0.22630534162619045</v>
+      </c>
+    </row>
+    <row r="56" spans="5:13" x14ac:dyDescent="0.35">
+      <c r="E56">
+        <f t="shared" si="15"/>
+        <v>24</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="16"/>
+        <v>30</v>
+      </c>
+      <c r="G56" s="10">
+        <v>105</v>
+      </c>
+      <c r="H56" s="11">
+        <v>204</v>
+      </c>
+      <c r="I56" s="11">
+        <v>210</v>
+      </c>
+      <c r="J56" s="10">
+        <f t="shared" si="17"/>
+        <v>338.64</v>
+      </c>
+      <c r="K56" s="11">
+        <f t="shared" si="18"/>
+        <v>348.59999999999997</v>
+      </c>
+      <c r="L56" s="11">
+        <f t="shared" ref="L56:M56" si="39">AC23</f>
+        <v>0.28841667191376597</v>
+      </c>
+      <c r="M56" s="11">
+        <f t="shared" si="39"/>
+        <v>0.24549330429356572</v>
+      </c>
+    </row>
+    <row r="57" spans="5:13" x14ac:dyDescent="0.35">
+      <c r="E57">
+        <f t="shared" si="15"/>
+        <v>26</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="16"/>
+        <v>31</v>
+      </c>
+      <c r="G57" s="10">
+        <v>110</v>
+      </c>
+      <c r="H57" s="11">
+        <v>206</v>
+      </c>
+      <c r="I57" s="11">
+        <v>211</v>
+      </c>
+      <c r="J57" s="10">
+        <f t="shared" si="17"/>
+        <v>341.96</v>
+      </c>
+      <c r="K57" s="11">
+        <f t="shared" si="18"/>
+        <v>350.26</v>
+      </c>
+      <c r="L57" s="11">
+        <f t="shared" ref="L57:M57" si="40">AC24</f>
+        <v>0.2943918465532504</v>
+      </c>
+      <c r="M57" s="11">
+        <f t="shared" si="40"/>
+        <v>0.2583129335637368</v>
+      </c>
+    </row>
+    <row r="58" spans="5:13" x14ac:dyDescent="0.35">
+      <c r="E58">
+        <f t="shared" si="15"/>
+        <v>27</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="16"/>
+        <v>32</v>
+      </c>
+      <c r="G58" s="10">
+        <v>115</v>
+      </c>
+      <c r="H58" s="11">
+        <v>207</v>
+      </c>
+      <c r="I58" s="11">
+        <v>212</v>
+      </c>
+      <c r="J58" s="10">
+        <f t="shared" si="17"/>
+        <v>343.62</v>
+      </c>
+      <c r="K58" s="11">
+        <f t="shared" si="18"/>
+        <v>351.91999999999996</v>
+      </c>
+      <c r="L58" s="11">
+        <f t="shared" ref="L58:M58" si="41">AC25</f>
+        <v>0.30778820015048997</v>
+      </c>
+      <c r="M58" s="11">
+        <f t="shared" si="41"/>
+        <v>0.27092488979724583</v>
+      </c>
+    </row>
+    <row r="59" spans="5:13" x14ac:dyDescent="0.35">
+      <c r="E59">
+        <f t="shared" si="15"/>
+        <v>28</v>
+      </c>
+      <c r="F59">
+        <f t="shared" si="16"/>
+        <v>33</v>
+      </c>
+      <c r="G59" s="10">
+        <v>120</v>
+      </c>
+      <c r="H59" s="11">
+        <v>208</v>
+      </c>
+      <c r="I59" s="11">
+        <v>213</v>
+      </c>
+      <c r="J59" s="10">
+        <f t="shared" si="17"/>
+        <v>345.28</v>
+      </c>
+      <c r="K59" s="11">
+        <f t="shared" si="18"/>
+        <v>353.58</v>
+      </c>
+      <c r="L59" s="11">
+        <f t="shared" ref="L59:M59" si="42">AC26</f>
+        <v>0.3209020084529689</v>
+      </c>
+      <c r="M59" s="11">
+        <f t="shared" si="42"/>
+        <v>0.28334617118633443</v>
+      </c>
+    </row>
+    <row r="60" spans="5:13" x14ac:dyDescent="0.35">
+      <c r="E60">
+        <f t="shared" si="15"/>
+        <v>29</v>
+      </c>
+      <c r="F60">
+        <f t="shared" si="16"/>
+        <v>34</v>
+      </c>
+      <c r="G60" s="10">
+        <v>125</v>
+      </c>
+      <c r="H60" s="11">
+        <v>209</v>
+      </c>
+      <c r="I60" s="11">
+        <v>214</v>
+      </c>
+      <c r="J60" s="10">
+        <f t="shared" si="17"/>
+        <v>346.94</v>
+      </c>
+      <c r="K60" s="11">
+        <f t="shared" si="18"/>
+        <v>355.24</v>
+      </c>
+      <c r="L60" s="11">
+        <f t="shared" ref="L60:M60" si="43">AC27</f>
+        <v>0.33375802536323124</v>
+      </c>
+      <c r="M60" s="11">
+        <f t="shared" si="43"/>
+        <v>0.2955964696913736</v>
+      </c>
+    </row>
+    <row r="61" spans="5:13" x14ac:dyDescent="0.35">
+      <c r="E61">
+        <f t="shared" si="15"/>
+        <v>30</v>
+      </c>
+      <c r="F61">
+        <f t="shared" si="16"/>
+        <v>35</v>
+      </c>
+      <c r="G61" s="10">
+        <v>130</v>
+      </c>
+      <c r="H61" s="11">
+        <v>210</v>
+      </c>
+      <c r="I61" s="11">
+        <v>215</v>
+      </c>
+      <c r="J61" s="10">
+        <f t="shared" si="17"/>
+        <v>348.59999999999997</v>
+      </c>
+      <c r="K61" s="11">
+        <f t="shared" si="18"/>
+        <v>356.9</v>
+      </c>
+      <c r="L61" s="11">
+        <f t="shared" ref="L61:M61" si="44">AC28</f>
+        <v>0.34638192096621484</v>
+      </c>
+      <c r="M61" s="11">
+        <f t="shared" si="44"/>
+        <v>0.30769751149758773</v>
+      </c>
+    </row>
+    <row r="62" spans="5:13" x14ac:dyDescent="0.35">
+      <c r="E62">
+        <f t="shared" si="15"/>
+        <v>32</v>
+      </c>
+      <c r="F62">
+        <f t="shared" si="16"/>
+        <v>36</v>
+      </c>
+      <c r="G62" s="12">
+        <v>135</v>
+      </c>
+      <c r="H62" s="13">
+        <v>212</v>
+      </c>
+      <c r="I62" s="13">
+        <v>216</v>
+      </c>
+      <c r="J62" s="12">
+        <f t="shared" si="17"/>
+        <v>351.91999999999996</v>
+      </c>
+      <c r="K62" s="13">
+        <f t="shared" si="18"/>
+        <v>358.56</v>
+      </c>
+      <c r="L62" s="13">
+        <f t="shared" ref="L62:M62" si="45">AC29</f>
+        <v>0.3506952689763535</v>
+      </c>
+      <c r="M62" s="13">
+        <f t="shared" si="45"/>
+        <v>0.31967249668293474</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>